<commit_message>
Fix: conversión de Numero_Mes y normalización de meses en artificial_lift_report
</commit_message>
<xml_diff>
--- a/als-salida.xlsx
+++ b/als-salida.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="85">
   <si>
     <t>WELL</t>
   </si>
@@ -100,9 +100,15 @@
     <t>Numero_Mes</t>
   </si>
   <si>
+    <t>ACAC-112</t>
+  </si>
+  <si>
     <t>ACAC-166</t>
   </si>
   <si>
+    <t>ACAD-095</t>
+  </si>
+  <si>
     <t>ACAE-082</t>
   </si>
   <si>
@@ -163,6 +169,9 @@
     <t>CLBA-006</t>
   </si>
   <si>
+    <t>CLBA-007R1</t>
+  </si>
+  <si>
     <t>CLBA-010H</t>
   </si>
   <si>
@@ -217,6 +226,9 @@
     <t>YLBA-030</t>
   </si>
   <si>
+    <t>YLBD-003</t>
+  </si>
+  <si>
     <t>YLBD-018</t>
   </si>
   <si>
@@ -227,6 +239,9 @@
   </si>
   <si>
     <t>YLBD-045H</t>
+  </si>
+  <si>
+    <t>Oct</t>
   </si>
   <si>
     <t>May</t>
@@ -611,7 +626,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AC45"/>
+  <dimension ref="A1:AC49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -705,7 +720,7 @@
     </row>
     <row r="2" spans="1:29">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
@@ -714,19 +729,19 @@
         <v>2025</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="E2">
-        <v>25184.02</v>
+        <v>12973.06</v>
       </c>
       <c r="F2">
-        <v>318432.7114</v>
+        <v>302399.9252000001</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>10239.5255</v>
       </c>
       <c r="H2">
-        <v>35498.4093</v>
+        <v>0</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -738,19 +753,19 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>78857.60000000001</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>25184.02</v>
+        <v>12973.06</v>
       </c>
       <c r="V2">
-        <v>318432.7114</v>
+        <v>302399.9252000001</v>
       </c>
       <c r="W2">
-        <v>0</v>
+        <v>10239.5255</v>
       </c>
       <c r="X2">
-        <v>35498.4093</v>
+        <v>0</v>
       </c>
       <c r="Y2">
         <v>0</v>
@@ -762,12 +777,12 @@
         <v>0</v>
       </c>
       <c r="AC2">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:29">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>29</v>
@@ -776,19 +791,19 @@
         <v>2025</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E3">
-        <v>17609.86</v>
+        <v>25184.02</v>
       </c>
       <c r="F3">
-        <v>243494.334</v>
+        <v>318432.7114</v>
       </c>
       <c r="G3">
-        <v>23610.8909</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>33707.7979</v>
+        <v>35498.4093</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -800,43 +815,19 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>81917.37000000001</v>
-      </c>
-      <c r="M3">
-        <v>39820.85</v>
-      </c>
-      <c r="N3">
-        <v>252738.5</v>
-      </c>
-      <c r="O3">
-        <v>21518.49</v>
-      </c>
-      <c r="P3">
-        <v>33647.97</v>
-      </c>
-      <c r="Q3">
-        <v>0</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>81917.37000000001</v>
+        <v>78857.60000000001</v>
       </c>
       <c r="U3">
-        <v>39820.85</v>
+        <v>25184.02</v>
       </c>
       <c r="V3">
-        <v>252738.5</v>
+        <v>318432.7114</v>
       </c>
       <c r="W3">
-        <v>21518.49</v>
+        <v>0</v>
       </c>
       <c r="X3">
-        <v>33647.97</v>
+        <v>35498.4093</v>
       </c>
       <c r="Y3">
         <v>0</v>
@@ -847,16 +838,13 @@
       <c r="AA3">
         <v>0</v>
       </c>
-      <c r="AB3">
-        <v>81917.37000000001</v>
-      </c>
       <c r="AC3">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:29">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
@@ -865,16 +853,16 @@
         <v>2025</v>
       </c>
       <c r="D4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E4">
-        <v>26603.62</v>
+        <v>18205.06</v>
       </c>
       <c r="F4">
-        <v>514831.7822</v>
+        <v>324144.4391</v>
       </c>
       <c r="G4">
-        <v>27028.2567</v>
+        <v>25164.239</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -883,46 +871,22 @@
         <v>0</v>
       </c>
       <c r="J4">
-        <v>72987.74000000001</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>141526.81</v>
-      </c>
-      <c r="M4">
-        <v>36289.75</v>
-      </c>
-      <c r="N4">
-        <v>454846.71</v>
-      </c>
-      <c r="O4">
-        <v>50340.94</v>
-      </c>
-      <c r="P4">
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>72987.74000000001</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>141526.81</v>
+        <v>0</v>
       </c>
       <c r="U4">
-        <v>36289.75</v>
+        <v>18205.06</v>
       </c>
       <c r="V4">
-        <v>454846.71</v>
+        <v>324144.4391</v>
       </c>
       <c r="W4">
-        <v>50340.94</v>
+        <v>25164.239</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -931,21 +895,18 @@
         <v>0</v>
       </c>
       <c r="Z4">
-        <v>72987.74000000001</v>
+        <v>0</v>
       </c>
       <c r="AA4">
         <v>0</v>
       </c>
-      <c r="AB4">
-        <v>141526.81</v>
-      </c>
       <c r="AC4">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:29">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>31</v>
@@ -954,19 +915,19 @@
         <v>2025</v>
       </c>
       <c r="D5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="E5">
-        <v>16058</v>
+        <v>17609.86</v>
       </c>
       <c r="F5">
-        <v>317342.6932</v>
+        <v>243494.334</v>
       </c>
       <c r="G5">
-        <v>26406.9175</v>
+        <v>23610.8909</v>
       </c>
       <c r="H5">
-        <v>36993.6621</v>
+        <v>33707.7979</v>
       </c>
       <c r="I5">
         <v>0</v>
@@ -978,19 +939,19 @@
         <v>0</v>
       </c>
       <c r="L5">
-        <v>83511.89999999999</v>
+        <v>81917.37000000001</v>
       </c>
       <c r="M5">
-        <v>38308.97</v>
+        <v>39820.85</v>
       </c>
       <c r="N5">
-        <v>258025.36</v>
+        <v>252738.5</v>
       </c>
       <c r="O5">
-        <v>0</v>
+        <v>21518.49</v>
       </c>
       <c r="P5">
-        <v>30826.26</v>
+        <v>33647.97</v>
       </c>
       <c r="Q5">
         <v>0</v>
@@ -1002,19 +963,19 @@
         <v>0</v>
       </c>
       <c r="T5">
-        <v>83812.86</v>
+        <v>81917.37000000001</v>
       </c>
       <c r="U5">
-        <v>38308.97</v>
+        <v>39820.85</v>
       </c>
       <c r="V5">
-        <v>258025.36</v>
+        <v>252738.5</v>
       </c>
       <c r="W5">
-        <v>0</v>
+        <v>21518.49</v>
       </c>
       <c r="X5">
-        <v>30826.26</v>
+        <v>33647.97</v>
       </c>
       <c r="Y5">
         <v>0</v>
@@ -1026,15 +987,15 @@
         <v>0</v>
       </c>
       <c r="AB5">
-        <v>83812.86</v>
+        <v>81917.37000000001</v>
       </c>
       <c r="AC5">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:29">
       <c r="A6" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -1043,40 +1004,40 @@
         <v>2025</v>
       </c>
       <c r="D6" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="E6">
-        <v>18755.46</v>
+        <v>26603.62</v>
       </c>
       <c r="F6">
-        <v>299802.0569</v>
+        <v>514831.7822</v>
       </c>
       <c r="G6">
-        <v>29513.6137</v>
+        <v>27028.2567</v>
       </c>
       <c r="H6">
-        <v>5712</v>
+        <v>0</v>
       </c>
       <c r="I6">
         <v>0</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>72987.74000000001</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>0</v>
+        <v>141526.81</v>
       </c>
       <c r="M6">
-        <v>28951.89</v>
+        <v>36289.75</v>
       </c>
       <c r="N6">
-        <v>297890.78</v>
+        <v>454846.71</v>
       </c>
       <c r="O6">
-        <v>25982.6</v>
+        <v>50340.94</v>
       </c>
       <c r="P6">
         <v>0</v>
@@ -1085,22 +1046,22 @@
         <v>0</v>
       </c>
       <c r="R6">
-        <v>0</v>
+        <v>72987.74000000001</v>
       </c>
       <c r="S6">
         <v>0</v>
       </c>
       <c r="T6">
-        <v>0</v>
+        <v>141526.81</v>
       </c>
       <c r="U6">
-        <v>28951.89</v>
+        <v>36289.75</v>
       </c>
       <c r="V6">
-        <v>297890.78</v>
+        <v>454846.71</v>
       </c>
       <c r="W6">
-        <v>25982.6</v>
+        <v>50340.94</v>
       </c>
       <c r="X6">
         <v>0</v>
@@ -1109,13 +1070,13 @@
         <v>0</v>
       </c>
       <c r="Z6">
-        <v>0</v>
+        <v>72987.74000000001</v>
       </c>
       <c r="AA6">
         <v>0</v>
       </c>
       <c r="AB6">
-        <v>0</v>
+        <v>141526.81</v>
       </c>
       <c r="AC6">
         <v>2</v>
@@ -1123,7 +1084,7 @@
     </row>
     <row r="7" spans="1:29">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -1132,19 +1093,19 @@
         <v>2025</v>
       </c>
       <c r="D7" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E7">
-        <v>19408.1</v>
+        <v>16058</v>
       </c>
       <c r="F7">
-        <v>28014.8339</v>
+        <v>317342.6932</v>
       </c>
       <c r="G7">
-        <v>55593.5105</v>
+        <v>26406.9175</v>
       </c>
       <c r="H7">
-        <v>36919.8225</v>
+        <v>36993.6621</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1156,19 +1117,19 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>0</v>
+        <v>83511.89999999999</v>
       </c>
       <c r="M7">
-        <v>27337.44</v>
+        <v>38308.97</v>
       </c>
       <c r="N7">
-        <v>281453.91</v>
+        <v>258025.36</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
-        <v>21807.01</v>
+        <v>30826.26</v>
       </c>
       <c r="Q7">
         <v>0</v>
@@ -1180,19 +1141,19 @@
         <v>0</v>
       </c>
       <c r="T7">
-        <v>0</v>
+        <v>83812.86</v>
       </c>
       <c r="U7">
-        <v>27337.44</v>
+        <v>38308.97</v>
       </c>
       <c r="V7">
-        <v>281453.91</v>
+        <v>258025.36</v>
       </c>
       <c r="W7">
         <v>0</v>
       </c>
       <c r="X7">
-        <v>21807.01</v>
+        <v>30826.26</v>
       </c>
       <c r="Y7">
         <v>0</v>
@@ -1204,15 +1165,15 @@
         <v>0</v>
       </c>
       <c r="AB7">
-        <v>0</v>
+        <v>83812.86</v>
       </c>
       <c r="AC7">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:29">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -1221,19 +1182,19 @@
         <v>2025</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>78</v>
       </c>
       <c r="E8">
-        <v>19027.18</v>
+        <v>18755.46</v>
       </c>
       <c r="F8">
-        <v>638405.0076</v>
+        <v>299802.0569</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>29513.6137</v>
       </c>
       <c r="H8">
-        <v>38027.4172</v>
+        <v>5712</v>
       </c>
       <c r="I8">
         <v>0</v>
@@ -1245,19 +1206,43 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <v>37198.7055</v>
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>28951.89</v>
+      </c>
+      <c r="N8">
+        <v>297890.78</v>
+      </c>
+      <c r="O8">
+        <v>25982.6</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>0</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>0</v>
       </c>
       <c r="U8">
-        <v>19027.18</v>
+        <v>28951.89</v>
       </c>
       <c r="V8">
-        <v>638405.0076</v>
+        <v>297890.78</v>
       </c>
       <c r="W8">
-        <v>0</v>
+        <v>25982.6</v>
       </c>
       <c r="X8">
-        <v>38027.4172</v>
+        <v>0</v>
       </c>
       <c r="Y8">
         <v>0</v>
@@ -1268,13 +1253,16 @@
       <c r="AA8">
         <v>0</v>
       </c>
+      <c r="AB8">
+        <v>0</v>
+      </c>
       <c r="AC8">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:29">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -1283,43 +1271,43 @@
         <v>2025</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E9">
-        <v>18205.06</v>
+        <v>19408.1</v>
       </c>
       <c r="F9">
-        <v>350421.9071</v>
+        <v>28014.8339</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>55593.5105</v>
       </c>
       <c r="H9">
-        <v>35996.8269</v>
+        <v>36919.8225</v>
       </c>
       <c r="I9">
         <v>0</v>
       </c>
       <c r="J9">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9">
-        <v>59030.4</v>
+        <v>0</v>
       </c>
       <c r="M9">
-        <v>34720.53</v>
+        <v>27337.44</v>
       </c>
       <c r="N9">
-        <v>271057.69</v>
+        <v>281453.91</v>
       </c>
       <c r="O9">
-        <v>19401.54</v>
+        <v>0</v>
       </c>
       <c r="P9">
-        <v>38992.08</v>
+        <v>21807.01</v>
       </c>
       <c r="Q9">
         <v>0</v>
@@ -1331,19 +1319,19 @@
         <v>0</v>
       </c>
       <c r="T9">
-        <v>59030.4</v>
+        <v>0</v>
       </c>
       <c r="U9">
-        <v>34720.53</v>
+        <v>27337.44</v>
       </c>
       <c r="V9">
-        <v>271057.69</v>
+        <v>281453.91</v>
       </c>
       <c r="W9">
-        <v>19401.54</v>
+        <v>0</v>
       </c>
       <c r="X9">
-        <v>38992.08</v>
+        <v>21807.01</v>
       </c>
       <c r="Y9">
         <v>0</v>
@@ -1355,15 +1343,15 @@
         <v>0</v>
       </c>
       <c r="AB9">
-        <v>59030.4</v>
+        <v>0</v>
       </c>
       <c r="AC9">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:29">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -1372,19 +1360,19 @@
         <v>2025</v>
       </c>
       <c r="D10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E10">
-        <v>13645.06</v>
+        <v>19027.18</v>
       </c>
       <c r="F10">
-        <v>299354.9628</v>
+        <v>638405.0076</v>
       </c>
       <c r="G10">
-        <v>12892.7891</v>
+        <v>0</v>
       </c>
       <c r="H10">
-        <v>18459.9112</v>
+        <v>38027.4172</v>
       </c>
       <c r="I10">
         <v>0</v>
@@ -1396,43 +1384,19 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10">
-        <v>19217.69</v>
-      </c>
-      <c r="N10">
-        <v>258930.56</v>
-      </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-      <c r="R10">
-        <v>0</v>
-      </c>
-      <c r="S10">
-        <v>0</v>
-      </c>
-      <c r="T10">
-        <v>0</v>
+        <v>37198.7055</v>
       </c>
       <c r="U10">
-        <v>19217.69</v>
+        <v>19027.18</v>
       </c>
       <c r="V10">
-        <v>258930.56</v>
+        <v>638405.0076</v>
       </c>
       <c r="W10">
         <v>0</v>
       </c>
       <c r="X10">
-        <v>0</v>
+        <v>38027.4172</v>
       </c>
       <c r="Y10">
         <v>0</v>
@@ -1443,16 +1407,13 @@
       <c r="AA10">
         <v>0</v>
       </c>
-      <c r="AB10">
-        <v>0</v>
-      </c>
       <c r="AC10">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -1461,43 +1422,67 @@
         <v>2025</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E11">
-        <v>22457.38</v>
+        <v>18205.06</v>
       </c>
       <c r="F11">
-        <v>294985.4912</v>
+        <v>350421.9071</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
       <c r="H11">
-        <v>0</v>
+        <v>35996.8269</v>
       </c>
       <c r="I11">
         <v>0</v>
       </c>
       <c r="J11">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="K11">
         <v>0</v>
       </c>
       <c r="L11">
-        <v>42006.49</v>
+        <v>59030.4</v>
+      </c>
+      <c r="M11">
+        <v>34720.53</v>
+      </c>
+      <c r="N11">
+        <v>271057.69</v>
+      </c>
+      <c r="O11">
+        <v>19401.54</v>
+      </c>
+      <c r="P11">
+        <v>38992.08</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>59030.4</v>
       </c>
       <c r="U11">
-        <v>22457.38</v>
+        <v>34720.53</v>
       </c>
       <c r="V11">
-        <v>294985.4912</v>
+        <v>271057.69</v>
       </c>
       <c r="W11">
-        <v>0</v>
+        <v>19401.54</v>
       </c>
       <c r="X11">
-        <v>0</v>
+        <v>38992.08</v>
       </c>
       <c r="Y11">
         <v>0</v>
@@ -1508,13 +1493,16 @@
       <c r="AA11">
         <v>0</v>
       </c>
+      <c r="AB11">
+        <v>59030.4</v>
+      </c>
       <c r="AC11">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -1523,19 +1511,19 @@
         <v>2025</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="E12">
-        <v>44610.66</v>
+        <v>13645.06</v>
       </c>
       <c r="F12">
-        <v>358194.8644</v>
+        <v>299354.9628</v>
       </c>
       <c r="G12">
-        <v>49129.3974</v>
+        <v>12892.7891</v>
       </c>
       <c r="H12">
-        <v>25843.8757</v>
+        <v>18459.9112</v>
       </c>
       <c r="I12">
         <v>0</v>
@@ -1544,22 +1532,46 @@
         <v>0</v>
       </c>
       <c r="K12">
-        <v>68709.94259999999</v>
+        <v>0</v>
       </c>
       <c r="L12">
         <v>0</v>
       </c>
+      <c r="M12">
+        <v>19217.69</v>
+      </c>
+      <c r="N12">
+        <v>258930.56</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
       <c r="U12">
-        <v>44610.66</v>
+        <v>19217.69</v>
       </c>
       <c r="V12">
-        <v>358194.8644</v>
+        <v>258930.56</v>
       </c>
       <c r="W12">
-        <v>49129.3974</v>
+        <v>0</v>
       </c>
       <c r="X12">
-        <v>25843.8757</v>
+        <v>0</v>
       </c>
       <c r="Y12">
         <v>0</v>
@@ -1568,15 +1580,18 @@
         <v>0</v>
       </c>
       <c r="AA12">
-        <v>68709.94259999999</v>
+        <v>0</v>
+      </c>
+      <c r="AB12">
+        <v>0</v>
       </c>
       <c r="AC12">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
@@ -1585,19 +1600,19 @@
         <v>2025</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E13">
-        <v>35264.5</v>
+        <v>22457.38</v>
       </c>
       <c r="F13">
-        <v>290894.2855</v>
+        <v>294985.4912</v>
       </c>
       <c r="G13">
-        <v>25630.2434</v>
+        <v>0</v>
       </c>
       <c r="H13">
-        <v>36735.2234</v>
+        <v>0</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1609,13 +1624,13 @@
         <v>0</v>
       </c>
       <c r="L13">
-        <v>41846.3631</v>
+        <v>42006.49</v>
       </c>
       <c r="M13">
-        <v>37882.47</v>
+        <v>40780.28000000001</v>
       </c>
       <c r="N13">
-        <v>278938.71</v>
+        <v>250365.09</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -1633,13 +1648,13 @@
         <v>0</v>
       </c>
       <c r="T13">
-        <v>41846.3631</v>
+        <v>42006.49</v>
       </c>
       <c r="U13">
-        <v>37882.47</v>
+        <v>40780.28000000001</v>
       </c>
       <c r="V13">
-        <v>278938.71</v>
+        <v>250365.09</v>
       </c>
       <c r="W13">
         <v>0</v>
@@ -1657,15 +1672,15 @@
         <v>0</v>
       </c>
       <c r="AB13">
-        <v>41846.3631</v>
+        <v>42006.49</v>
       </c>
       <c r="AC13">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="1">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
@@ -1674,19 +1689,19 @@
         <v>2025</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="E14">
-        <v>21182.46</v>
+        <v>44610.66</v>
       </c>
       <c r="F14">
-        <v>516832.16</v>
+        <v>358194.8644</v>
       </c>
       <c r="G14">
-        <v>41714.5254</v>
+        <v>49129.3974</v>
       </c>
       <c r="H14">
-        <v>36735.2234</v>
+        <v>25843.8757</v>
       </c>
       <c r="I14">
         <v>0</v>
@@ -1695,22 +1710,22 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>5293.4</v>
+        <v>68709.94259999999</v>
       </c>
       <c r="L14">
-        <v>199012.794</v>
+        <v>0</v>
       </c>
       <c r="M14">
-        <v>29506.7</v>
+        <v>24406.71</v>
       </c>
       <c r="N14">
-        <v>455228.52</v>
+        <v>340968.83</v>
       </c>
       <c r="O14">
-        <v>2181.06</v>
+        <v>5162.22</v>
       </c>
       <c r="P14">
-        <v>0</v>
+        <v>22756.23</v>
       </c>
       <c r="Q14">
         <v>0</v>
@@ -1719,22 +1734,22 @@
         <v>0</v>
       </c>
       <c r="S14">
-        <v>64902.09</v>
+        <v>115340</v>
       </c>
       <c r="T14">
-        <v>199012.794</v>
+        <v>0</v>
       </c>
       <c r="U14">
-        <v>29506.7</v>
+        <v>24406.71</v>
       </c>
       <c r="V14">
-        <v>455228.52</v>
+        <v>340968.83</v>
       </c>
       <c r="W14">
-        <v>2181.06</v>
+        <v>5162.22</v>
       </c>
       <c r="X14">
-        <v>0</v>
+        <v>22756.23</v>
       </c>
       <c r="Y14">
         <v>0</v>
@@ -1743,36 +1758,36 @@
         <v>0</v>
       </c>
       <c r="AA14">
-        <v>64902.09</v>
+        <v>115340</v>
       </c>
       <c r="AB14">
-        <v>199012.794</v>
+        <v>0</v>
       </c>
       <c r="AC14">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="1">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C15">
         <v>2025</v>
       </c>
       <c r="D15" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="E15">
-        <v>18397.06</v>
+        <v>35264.5</v>
       </c>
       <c r="F15">
-        <v>326646.9343</v>
+        <v>290894.2855</v>
       </c>
       <c r="G15">
-        <v>24329.9319</v>
+        <v>25630.2434</v>
       </c>
       <c r="H15">
         <v>36735.2234</v>
@@ -1787,19 +1802,43 @@
         <v>0</v>
       </c>
       <c r="L15">
-        <v>36863.1</v>
+        <v>41846.3631</v>
+      </c>
+      <c r="M15">
+        <v>37882.47</v>
+      </c>
+      <c r="N15">
+        <v>278938.71</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>41846.3631</v>
       </c>
       <c r="U15">
-        <v>18397.06</v>
+        <v>37882.47</v>
       </c>
       <c r="V15">
-        <v>326646.9343</v>
+        <v>278938.71</v>
       </c>
       <c r="W15">
-        <v>24329.9319</v>
+        <v>0</v>
       </c>
       <c r="X15">
-        <v>36735.2234</v>
+        <v>0</v>
       </c>
       <c r="Y15">
         <v>0</v>
@@ -1810,16 +1849,19 @@
       <c r="AA15">
         <v>0</v>
       </c>
+      <c r="AB15">
+        <v>41846.3631</v>
+      </c>
       <c r="AC15">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="1">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C16">
         <v>2025</v>
@@ -1828,16 +1870,16 @@
         <v>77</v>
       </c>
       <c r="E16">
-        <v>25142.02</v>
+        <v>21182.46</v>
       </c>
       <c r="F16">
-        <v>277188.6893</v>
+        <v>516832.16</v>
       </c>
       <c r="G16">
-        <v>24698.2346</v>
+        <v>41714.5254</v>
       </c>
       <c r="H16">
-        <v>35406.1098</v>
+        <v>36735.2234</v>
       </c>
       <c r="I16">
         <v>0</v>
@@ -1846,19 +1888,19 @@
         <v>0</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>5293.4</v>
       </c>
       <c r="L16">
-        <v>173339.58</v>
+        <v>199012.794</v>
       </c>
       <c r="M16">
-        <v>28089.2</v>
+        <v>29506.7</v>
       </c>
       <c r="N16">
-        <v>160763.94</v>
+        <v>455228.52</v>
       </c>
       <c r="O16">
-        <v>0</v>
+        <v>2181.06</v>
       </c>
       <c r="P16">
         <v>0</v>
@@ -1870,19 +1912,19 @@
         <v>0</v>
       </c>
       <c r="S16">
-        <v>0</v>
+        <v>64902.09</v>
       </c>
       <c r="T16">
-        <v>173339.58</v>
+        <v>199012.794</v>
       </c>
       <c r="U16">
-        <v>28089.2</v>
+        <v>29506.7</v>
       </c>
       <c r="V16">
-        <v>160763.94</v>
+        <v>455228.52</v>
       </c>
       <c r="W16">
-        <v>0</v>
+        <v>2181.06</v>
       </c>
       <c r="X16">
         <v>0</v>
@@ -1894,18 +1936,18 @@
         <v>0</v>
       </c>
       <c r="AA16">
-        <v>0</v>
+        <v>64902.09</v>
       </c>
       <c r="AB16">
-        <v>173339.58</v>
+        <v>199012.794</v>
       </c>
       <c r="AC16">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
@@ -1914,19 +1956,19 @@
         <v>2025</v>
       </c>
       <c r="D17" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="E17">
-        <v>15006.48</v>
+        <v>18397.06</v>
       </c>
       <c r="F17">
-        <v>324866.7652</v>
+        <v>326646.9343</v>
       </c>
       <c r="G17">
-        <v>38730.0079</v>
+        <v>24329.9319</v>
       </c>
       <c r="H17">
-        <v>39190.3916</v>
+        <v>36735.2234</v>
       </c>
       <c r="I17">
         <v>0</v>
@@ -1938,19 +1980,43 @@
         <v>0</v>
       </c>
       <c r="L17">
-        <v>0</v>
+        <v>36863.1</v>
+      </c>
+      <c r="M17">
+        <v>36093.04</v>
+      </c>
+      <c r="N17">
+        <v>324824.84</v>
+      </c>
+      <c r="O17">
+        <v>7421.05</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>36863.1</v>
       </c>
       <c r="U17">
-        <v>15006.48</v>
+        <v>36093.04</v>
       </c>
       <c r="V17">
-        <v>324866.7652</v>
+        <v>324824.84</v>
       </c>
       <c r="W17">
-        <v>38730.0079</v>
+        <v>7421.05</v>
       </c>
       <c r="X17">
-        <v>39190.3916</v>
+        <v>0</v>
       </c>
       <c r="Y17">
         <v>0</v>
@@ -1960,6 +2026,9 @@
       </c>
       <c r="AA17">
         <v>0</v>
+      </c>
+      <c r="AB17">
+        <v>36863.1</v>
       </c>
       <c r="AC17">
         <v>9</v>
@@ -1967,7 +2036,7 @@
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
@@ -1976,19 +2045,19 @@
         <v>2025</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E18">
-        <v>26099.62</v>
+        <v>25142.02</v>
       </c>
       <c r="F18">
-        <v>278579.4218</v>
+        <v>277188.6893</v>
       </c>
       <c r="G18">
-        <v>26251.5827</v>
+        <v>24698.2346</v>
       </c>
       <c r="H18">
-        <v>0</v>
+        <v>35406.1098</v>
       </c>
       <c r="I18">
         <v>0</v>
@@ -2000,13 +2069,13 @@
         <v>0</v>
       </c>
       <c r="L18">
-        <v>29992.31</v>
+        <v>173339.58</v>
       </c>
       <c r="M18">
-        <v>24651.29</v>
+        <v>28089.2</v>
       </c>
       <c r="N18">
-        <v>267851.66</v>
+        <v>160763.94</v>
       </c>
       <c r="O18">
         <v>0</v>
@@ -2024,13 +2093,13 @@
         <v>0</v>
       </c>
       <c r="T18">
-        <v>29992.31</v>
+        <v>173339.58</v>
       </c>
       <c r="U18">
-        <v>24651.29</v>
+        <v>28089.2</v>
       </c>
       <c r="V18">
-        <v>267851.66</v>
+        <v>160763.94</v>
       </c>
       <c r="W18">
         <v>0</v>
@@ -2048,7 +2117,7 @@
         <v>0</v>
       </c>
       <c r="AB18">
-        <v>29992.31</v>
+        <v>173339.58</v>
       </c>
       <c r="AC18">
         <v>1</v>
@@ -2056,7 +2125,7 @@
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
@@ -2065,19 +2134,19 @@
         <v>2025</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="E19">
-        <v>27006.82</v>
+        <v>15006.48</v>
       </c>
       <c r="F19">
-        <v>264147.2883</v>
+        <v>324866.7652</v>
       </c>
       <c r="G19">
-        <v>27649.596</v>
+        <v>38730.0079</v>
       </c>
       <c r="H19">
-        <v>0</v>
+        <v>39190.3916</v>
       </c>
       <c r="I19">
         <v>0</v>
@@ -2089,19 +2158,19 @@
         <v>0</v>
       </c>
       <c r="L19">
-        <v>64312.56099999999</v>
+        <v>0</v>
       </c>
       <c r="M19">
-        <v>33999.38</v>
+        <v>50944.75</v>
       </c>
       <c r="N19">
-        <v>278850.94</v>
+        <v>288251.2</v>
       </c>
       <c r="O19">
-        <v>0</v>
+        <v>9109.799999999999</v>
       </c>
       <c r="P19">
-        <v>0</v>
+        <v>16977.39</v>
       </c>
       <c r="Q19">
         <v>0</v>
@@ -2113,19 +2182,19 @@
         <v>0</v>
       </c>
       <c r="T19">
-        <v>64312.56099999999</v>
+        <v>0</v>
       </c>
       <c r="U19">
-        <v>33999.38</v>
+        <v>50944.75</v>
       </c>
       <c r="V19">
-        <v>278850.94</v>
+        <v>288251.2</v>
       </c>
       <c r="W19">
-        <v>0</v>
+        <v>9109.799999999999</v>
       </c>
       <c r="X19">
-        <v>0</v>
+        <v>16977.39</v>
       </c>
       <c r="Y19">
         <v>0</v>
@@ -2137,15 +2206,15 @@
         <v>0</v>
       </c>
       <c r="AB19">
-        <v>64312.56099999999</v>
+        <v>0</v>
       </c>
       <c r="AC19">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="1">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
@@ -2154,19 +2223,19 @@
         <v>2025</v>
       </c>
       <c r="D20" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E20">
-        <v>18896.26</v>
+        <v>26099.62</v>
       </c>
       <c r="F20">
-        <v>320793.0784</v>
+        <v>278579.4218</v>
       </c>
       <c r="G20">
-        <v>27028.2567</v>
+        <v>26251.5827</v>
       </c>
       <c r="H20">
-        <v>10686.4527</v>
+        <v>0</v>
       </c>
       <c r="I20">
         <v>0</v>
@@ -2178,19 +2247,43 @@
         <v>0</v>
       </c>
       <c r="L20">
-        <v>0</v>
+        <v>29992.31</v>
+      </c>
+      <c r="M20">
+        <v>24651.29</v>
+      </c>
+      <c r="N20">
+        <v>267851.66</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>0</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>29992.31</v>
       </c>
       <c r="U20">
-        <v>18896.26</v>
+        <v>24651.29</v>
       </c>
       <c r="V20">
-        <v>320793.0784</v>
+        <v>267851.66</v>
       </c>
       <c r="W20">
-        <v>27028.2567</v>
+        <v>0</v>
       </c>
       <c r="X20">
-        <v>10686.4527</v>
+        <v>0</v>
       </c>
       <c r="Y20">
         <v>0</v>
@@ -2201,13 +2294,16 @@
       <c r="AA20">
         <v>0</v>
       </c>
+      <c r="AB20">
+        <v>29992.31</v>
+      </c>
       <c r="AC20">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
@@ -2216,16 +2312,16 @@
         <v>2025</v>
       </c>
       <c r="D21" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E21">
-        <v>17000</v>
+        <v>27006.82</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>264147.2883</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>27649.596</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -2240,13 +2336,37 @@
         <v>0</v>
       </c>
       <c r="L21">
-        <v>0</v>
+        <v>64312.56099999999</v>
+      </c>
+      <c r="M21">
+        <v>33999.38</v>
+      </c>
+      <c r="N21">
+        <v>278850.94</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>0</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>64312.56099999999</v>
       </c>
       <c r="U21">
-        <v>17000</v>
+        <v>33999.38</v>
       </c>
       <c r="V21">
-        <v>0</v>
+        <v>278850.94</v>
       </c>
       <c r="W21">
         <v>0</v>
@@ -2263,13 +2383,16 @@
       <c r="AA21">
         <v>0</v>
       </c>
+      <c r="AB21">
+        <v>64312.56099999999</v>
+      </c>
       <c r="AC21">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
@@ -2278,19 +2401,19 @@
         <v>2025</v>
       </c>
       <c r="D22" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E22">
-        <v>26563.62</v>
+        <v>18896.26</v>
       </c>
       <c r="F22">
-        <v>283269.233</v>
+        <v>320793.0784</v>
       </c>
       <c r="G22">
-        <v>25785.5783</v>
+        <v>27028.2567</v>
       </c>
       <c r="H22">
-        <v>36919.8225</v>
+        <v>10686.4527</v>
       </c>
       <c r="I22">
         <v>0</v>
@@ -2302,43 +2425,19 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <v>18450</v>
-      </c>
-      <c r="M22">
-        <v>32674.29</v>
-      </c>
-      <c r="N22">
-        <v>290087.79</v>
-      </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-      <c r="P22">
-        <v>16697.25</v>
-      </c>
-      <c r="Q22">
-        <v>0</v>
-      </c>
-      <c r="R22">
-        <v>0</v>
-      </c>
-      <c r="S22">
-        <v>0</v>
-      </c>
-      <c r="T22">
-        <v>18450</v>
+        <v>0</v>
       </c>
       <c r="U22">
-        <v>32674.29</v>
+        <v>18896.26</v>
       </c>
       <c r="V22">
-        <v>290087.79</v>
+        <v>320793.0784</v>
       </c>
       <c r="W22">
-        <v>0</v>
+        <v>27028.2567</v>
       </c>
       <c r="X22">
-        <v>16697.25</v>
+        <v>10686.4527</v>
       </c>
       <c r="Y22">
         <v>0</v>
@@ -2349,16 +2448,13 @@
       <c r="AA22">
         <v>0</v>
       </c>
-      <c r="AB22">
-        <v>18450</v>
-      </c>
       <c r="AC22">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
@@ -2367,13 +2463,13 @@
         <v>2025</v>
       </c>
       <c r="D23" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="E23">
-        <v>18812.78</v>
+        <v>17000</v>
       </c>
       <c r="F23">
-        <v>591541.1514</v>
+        <v>0</v>
       </c>
       <c r="G23">
         <v>0</v>
@@ -2388,43 +2484,19 @@
         <v>0</v>
       </c>
       <c r="K23">
-        <v>95464.1189</v>
+        <v>0</v>
       </c>
       <c r="L23">
-        <v>19227.3628</v>
-      </c>
-      <c r="M23">
-        <v>23508.78</v>
-      </c>
-      <c r="N23">
-        <v>568269.17</v>
-      </c>
-      <c r="O23">
-        <v>2615.02</v>
-      </c>
-      <c r="P23">
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <v>0</v>
-      </c>
-      <c r="R23">
-        <v>36493.87</v>
-      </c>
-      <c r="S23">
-        <v>90840</v>
-      </c>
-      <c r="T23">
-        <v>19719.56</v>
+        <v>0</v>
       </c>
       <c r="U23">
-        <v>23508.78</v>
+        <v>17000</v>
       </c>
       <c r="V23">
-        <v>568269.17</v>
+        <v>0</v>
       </c>
       <c r="W23">
-        <v>2615.02</v>
+        <v>0</v>
       </c>
       <c r="X23">
         <v>0</v>
@@ -2433,21 +2505,18 @@
         <v>0</v>
       </c>
       <c r="Z23">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="AA23">
-        <v>90840</v>
-      </c>
-      <c r="AB23">
-        <v>19719.56</v>
+        <v>0</v>
       </c>
       <c r="AC23">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="1">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
         <v>49</v>
@@ -2456,87 +2525,87 @@
         <v>2025</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E24">
-        <v>18963.92</v>
+        <v>26563.62</v>
       </c>
       <c r="F24">
-        <v>267383.277</v>
+        <v>283269.233</v>
       </c>
       <c r="G24">
-        <v>25093.7551</v>
+        <v>25785.5783</v>
       </c>
       <c r="H24">
-        <v>0</v>
+        <v>36919.8225</v>
       </c>
       <c r="I24">
         <v>0</v>
       </c>
       <c r="J24">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="K24">
         <v>0</v>
       </c>
       <c r="L24">
-        <v>0</v>
+        <v>18450</v>
       </c>
       <c r="M24">
-        <v>29758.22</v>
+        <v>32674.29</v>
       </c>
       <c r="N24">
-        <v>245114.65</v>
+        <v>290087.79</v>
       </c>
       <c r="O24">
-        <v>6805.46</v>
+        <v>0</v>
       </c>
       <c r="P24">
-        <v>10800.63</v>
+        <v>16697.25</v>
       </c>
       <c r="Q24">
         <v>0</v>
       </c>
       <c r="R24">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="S24">
         <v>0</v>
       </c>
       <c r="T24">
-        <v>0</v>
+        <v>18450</v>
       </c>
       <c r="U24">
-        <v>29758.22</v>
+        <v>32674.29</v>
       </c>
       <c r="V24">
-        <v>245114.65</v>
+        <v>290087.79</v>
       </c>
       <c r="W24">
-        <v>6805.46</v>
+        <v>0</v>
       </c>
       <c r="X24">
-        <v>10800.63</v>
+        <v>16697.25</v>
       </c>
       <c r="Y24">
         <v>0</v>
       </c>
       <c r="Z24">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="AA24">
         <v>0</v>
       </c>
       <c r="AB24">
-        <v>0</v>
+        <v>18450</v>
       </c>
       <c r="AC24">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="1">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
@@ -2545,19 +2614,19 @@
         <v>2025</v>
       </c>
       <c r="D25" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E25">
-        <v>16590.18</v>
+        <v>18812.78</v>
       </c>
       <c r="F25">
-        <v>327010.7217</v>
+        <v>591541.1514</v>
       </c>
       <c r="G25">
-        <v>25630.2434</v>
+        <v>0</v>
       </c>
       <c r="H25">
-        <v>36402.945</v>
+        <v>0</v>
       </c>
       <c r="I25">
         <v>0</v>
@@ -2566,58 +2635,58 @@
         <v>0</v>
       </c>
       <c r="K25">
-        <v>0</v>
+        <v>95464.1189</v>
       </c>
       <c r="L25">
-        <v>0</v>
+        <v>19227.3628</v>
       </c>
       <c r="M25">
-        <v>21705.25</v>
+        <v>23508.78</v>
       </c>
       <c r="N25">
-        <v>287071.98</v>
+        <v>568269.17</v>
       </c>
       <c r="O25">
-        <v>0</v>
+        <v>2615.02</v>
       </c>
       <c r="P25">
-        <v>36194.4</v>
+        <v>0</v>
       </c>
       <c r="Q25">
         <v>0</v>
       </c>
       <c r="R25">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="S25">
-        <v>0</v>
+        <v>90840</v>
       </c>
       <c r="T25">
-        <v>0</v>
+        <v>19719.56</v>
       </c>
       <c r="U25">
-        <v>21705.25</v>
+        <v>23508.78</v>
       </c>
       <c r="V25">
-        <v>287071.98</v>
+        <v>568269.17</v>
       </c>
       <c r="W25">
-        <v>0</v>
+        <v>2615.02</v>
       </c>
       <c r="X25">
-        <v>36194.4</v>
+        <v>0</v>
       </c>
       <c r="Y25">
         <v>0</v>
       </c>
       <c r="Z25">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="AA25">
-        <v>0</v>
+        <v>90840</v>
       </c>
       <c r="AB25">
-        <v>0</v>
+        <v>19719.56</v>
       </c>
       <c r="AC25">
         <v>3</v>
@@ -2625,7 +2694,7 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="1">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -2634,19 +2703,19 @@
         <v>2025</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E26">
-        <v>18460.42</v>
+        <v>21300</v>
       </c>
       <c r="F26">
-        <v>281664.89</v>
+        <v>303500</v>
       </c>
       <c r="G26">
-        <v>25785.58</v>
+        <v>39800</v>
       </c>
       <c r="H26">
-        <v>36978.89</v>
+        <v>0</v>
       </c>
       <c r="I26">
         <v>0</v>
@@ -2655,43 +2724,19 @@
         <v>0</v>
       </c>
       <c r="K26">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="L26">
         <v>0</v>
       </c>
-      <c r="M26">
-        <v>28420.94</v>
-      </c>
-      <c r="N26">
-        <v>239742.97</v>
-      </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>0</v>
-      </c>
-      <c r="R26">
-        <v>0</v>
-      </c>
-      <c r="S26">
-        <v>0</v>
-      </c>
-      <c r="T26">
-        <v>0</v>
-      </c>
       <c r="U26">
-        <v>28420.94</v>
+        <v>21300</v>
       </c>
       <c r="V26">
-        <v>239742.97</v>
+        <v>303500</v>
       </c>
       <c r="W26">
-        <v>0</v>
+        <v>39800</v>
       </c>
       <c r="X26">
         <v>0</v>
@@ -2703,18 +2748,15 @@
         <v>0</v>
       </c>
       <c r="AA26">
-        <v>0</v>
-      </c>
-      <c r="AB26">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="AC26">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
@@ -2723,87 +2765,87 @@
         <v>2025</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E27">
-        <v>18541.06</v>
+        <v>18963.92</v>
       </c>
       <c r="F27">
-        <v>319530.8217</v>
+        <v>267383.277</v>
       </c>
       <c r="G27">
-        <v>36708.3923</v>
+        <v>25093.7551</v>
       </c>
       <c r="H27">
-        <v>37289.0207</v>
+        <v>0</v>
       </c>
       <c r="I27">
         <v>0</v>
       </c>
       <c r="J27">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="K27">
-        <v>5373.2</v>
+        <v>0</v>
       </c>
       <c r="L27">
-        <v>82632.71000000001</v>
+        <v>0</v>
       </c>
       <c r="M27">
-        <v>24335.07</v>
+        <v>29758.22</v>
       </c>
       <c r="N27">
-        <v>247385.28</v>
+        <v>245114.65</v>
       </c>
       <c r="O27">
-        <v>0</v>
+        <v>6805.46</v>
       </c>
       <c r="P27">
-        <v>6678.9</v>
+        <v>10800.63</v>
       </c>
       <c r="Q27">
         <v>0</v>
       </c>
       <c r="R27">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="S27">
         <v>0</v>
       </c>
       <c r="T27">
-        <v>82632.71000000001</v>
+        <v>0</v>
       </c>
       <c r="U27">
-        <v>24335.07</v>
+        <v>29758.22</v>
       </c>
       <c r="V27">
-        <v>247385.28</v>
+        <v>245114.65</v>
       </c>
       <c r="W27">
-        <v>0</v>
+        <v>6805.46</v>
       </c>
       <c r="X27">
-        <v>6678.9</v>
+        <v>10800.63</v>
       </c>
       <c r="Y27">
         <v>0</v>
       </c>
       <c r="Z27">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="AA27">
         <v>0</v>
       </c>
       <c r="AB27">
-        <v>82632.71000000001</v>
+        <v>0</v>
       </c>
       <c r="AC27">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="1">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -2815,16 +2857,16 @@
         <v>79</v>
       </c>
       <c r="E28">
-        <v>14932.88</v>
+        <v>16590.18</v>
       </c>
       <c r="F28">
-        <v>262147.1729</v>
+        <v>327010.7217</v>
       </c>
       <c r="G28">
-        <v>0</v>
+        <v>25630.2434</v>
       </c>
       <c r="H28">
-        <v>0</v>
+        <v>36402.945</v>
       </c>
       <c r="I28">
         <v>0</v>
@@ -2833,22 +2875,22 @@
         <v>0</v>
       </c>
       <c r="K28">
-        <v>5376</v>
+        <v>0</v>
       </c>
       <c r="L28">
         <v>0</v>
       </c>
       <c r="M28">
-        <v>22202.17</v>
+        <v>21705.25</v>
       </c>
       <c r="N28">
-        <v>232396.83</v>
+        <v>287071.98</v>
       </c>
       <c r="O28">
-        <v>3310.93</v>
+        <v>0</v>
       </c>
       <c r="P28">
-        <v>0</v>
+        <v>36194.4</v>
       </c>
       <c r="Q28">
         <v>0</v>
@@ -2863,16 +2905,16 @@
         <v>0</v>
       </c>
       <c r="U28">
-        <v>22202.17</v>
+        <v>21705.25</v>
       </c>
       <c r="V28">
-        <v>232396.83</v>
+        <v>287071.98</v>
       </c>
       <c r="W28">
-        <v>3310.93</v>
+        <v>0</v>
       </c>
       <c r="X28">
-        <v>0</v>
+        <v>36194.4</v>
       </c>
       <c r="Y28">
         <v>0</v>
@@ -2887,12 +2929,12 @@
         <v>0</v>
       </c>
       <c r="AC28">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -2901,19 +2943,19 @@
         <v>2025</v>
       </c>
       <c r="D29" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="E29">
-        <v>16058</v>
+        <v>18460.42</v>
       </c>
       <c r="F29">
-        <v>317342.6932</v>
+        <v>281664.89</v>
       </c>
       <c r="G29">
-        <v>26406.9175</v>
+        <v>25785.58</v>
       </c>
       <c r="H29">
-        <v>36993.6621</v>
+        <v>36978.89</v>
       </c>
       <c r="I29">
         <v>0</v>
@@ -2925,16 +2967,16 @@
         <v>0</v>
       </c>
       <c r="L29">
-        <v>14106.87</v>
+        <v>0</v>
       </c>
       <c r="M29">
-        <v>31949.91</v>
+        <v>28420.94</v>
       </c>
       <c r="N29">
-        <v>264422.99</v>
+        <v>239742.97</v>
       </c>
       <c r="O29">
-        <v>6589.74</v>
+        <v>0</v>
       </c>
       <c r="P29">
         <v>0</v>
@@ -2949,16 +2991,16 @@
         <v>0</v>
       </c>
       <c r="T29">
-        <v>14106.87</v>
+        <v>0</v>
       </c>
       <c r="U29">
-        <v>31949.91</v>
+        <v>28420.94</v>
       </c>
       <c r="V29">
-        <v>264422.99</v>
+        <v>239742.97</v>
       </c>
       <c r="W29">
-        <v>6589.74</v>
+        <v>0</v>
       </c>
       <c r="X29">
         <v>0</v>
@@ -2973,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="AB29">
-        <v>14106.87</v>
+        <v>0</v>
       </c>
       <c r="AC29">
         <v>6</v>
@@ -2981,7 +3023,7 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B30" t="s">
         <v>55</v>
@@ -2990,19 +3032,19 @@
         <v>2025</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E30">
-        <v>15265.68</v>
+        <v>18541.06</v>
       </c>
       <c r="F30">
-        <v>311352.2643</v>
+        <v>319530.8217</v>
       </c>
       <c r="G30">
-        <v>26406.9175</v>
+        <v>36708.3923</v>
       </c>
       <c r="H30">
-        <v>0</v>
+        <v>37289.0207</v>
       </c>
       <c r="I30">
         <v>0</v>
@@ -3011,22 +3053,22 @@
         <v>0</v>
       </c>
       <c r="K30">
-        <v>0</v>
+        <v>5373.2</v>
       </c>
       <c r="L30">
-        <v>0</v>
+        <v>82632.71000000001</v>
       </c>
       <c r="M30">
-        <v>34725.64</v>
+        <v>24335.07</v>
       </c>
       <c r="N30">
-        <v>314368.92</v>
+        <v>247385.28</v>
       </c>
       <c r="O30">
         <v>0</v>
       </c>
       <c r="P30">
-        <v>0</v>
+        <v>6678.9</v>
       </c>
       <c r="Q30">
         <v>0</v>
@@ -3038,19 +3080,19 @@
         <v>0</v>
       </c>
       <c r="T30">
-        <v>0</v>
+        <v>82632.71000000001</v>
       </c>
       <c r="U30">
-        <v>34725.64</v>
+        <v>24335.07</v>
       </c>
       <c r="V30">
-        <v>314368.92</v>
+        <v>247385.28</v>
       </c>
       <c r="W30">
         <v>0</v>
       </c>
       <c r="X30">
-        <v>0</v>
+        <v>6678.9</v>
       </c>
       <c r="Y30">
         <v>0</v>
@@ -3062,15 +3104,15 @@
         <v>0</v>
       </c>
       <c r="AB30">
-        <v>0</v>
+        <v>82632.71000000001</v>
       </c>
       <c r="AC30">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="1">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
@@ -3079,13 +3121,13 @@
         <v>2025</v>
       </c>
       <c r="D31" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="E31">
-        <v>20558.98</v>
+        <v>14932.88</v>
       </c>
       <c r="F31">
-        <v>300178.145</v>
+        <v>262147.1729</v>
       </c>
       <c r="G31">
         <v>0</v>
@@ -3097,22 +3139,46 @@
         <v>0</v>
       </c>
       <c r="J31">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="K31">
-        <v>0</v>
+        <v>5376</v>
       </c>
       <c r="L31">
         <v>0</v>
       </c>
+      <c r="M31">
+        <v>22202.17</v>
+      </c>
+      <c r="N31">
+        <v>231965.51</v>
+      </c>
+      <c r="O31">
+        <v>3310.93</v>
+      </c>
+      <c r="P31">
+        <v>0</v>
+      </c>
+      <c r="Q31">
+        <v>0</v>
+      </c>
+      <c r="R31">
+        <v>0</v>
+      </c>
+      <c r="S31">
+        <v>0</v>
+      </c>
+      <c r="T31">
+        <v>0</v>
+      </c>
       <c r="U31">
-        <v>20558.98</v>
+        <v>22202.17</v>
       </c>
       <c r="V31">
-        <v>300178.145</v>
+        <v>231965.51</v>
       </c>
       <c r="W31">
-        <v>0</v>
+        <v>3310.93</v>
       </c>
       <c r="X31">
         <v>0</v>
@@ -3121,18 +3187,21 @@
         <v>0</v>
       </c>
       <c r="Z31">
-        <v>36493.87</v>
+        <v>0</v>
       </c>
       <c r="AA31">
         <v>0</v>
       </c>
+      <c r="AB31">
+        <v>0</v>
+      </c>
       <c r="AC31">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="1">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>57</v>
@@ -3141,22 +3210,22 @@
         <v>2025</v>
       </c>
       <c r="D32" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E32">
-        <v>80000</v>
+        <v>16058</v>
       </c>
       <c r="F32">
-        <v>120000</v>
+        <v>317342.6932</v>
       </c>
       <c r="G32">
-        <v>0</v>
+        <v>26406.9175</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>36993.6621</v>
       </c>
       <c r="I32">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="J32">
         <v>0</v>
@@ -3165,22 +3234,46 @@
         <v>0</v>
       </c>
       <c r="L32">
-        <v>22674.42</v>
+        <v>14106.87</v>
+      </c>
+      <c r="M32">
+        <v>31949.91</v>
+      </c>
+      <c r="N32">
+        <v>264422.99</v>
+      </c>
+      <c r="O32">
+        <v>6589.74</v>
+      </c>
+      <c r="P32">
+        <v>0</v>
+      </c>
+      <c r="Q32">
+        <v>0</v>
+      </c>
+      <c r="R32">
+        <v>0</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>14106.87</v>
       </c>
       <c r="U32">
-        <v>80000</v>
+        <v>31949.91</v>
       </c>
       <c r="V32">
-        <v>120000</v>
+        <v>264422.99</v>
       </c>
       <c r="W32">
-        <v>0</v>
+        <v>6589.74</v>
       </c>
       <c r="X32">
         <v>0</v>
       </c>
       <c r="Y32">
-        <v>35000</v>
+        <v>0</v>
       </c>
       <c r="Z32">
         <v>0</v>
@@ -3188,13 +3281,16 @@
       <c r="AA32">
         <v>0</v>
       </c>
+      <c r="AB32">
+        <v>14106.87</v>
+      </c>
       <c r="AC32">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="1">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B33" t="s">
         <v>58</v>
@@ -3203,16 +3299,16 @@
         <v>2025</v>
       </c>
       <c r="D33" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="E33">
-        <v>14668.56</v>
+        <v>15265.68</v>
       </c>
       <c r="F33">
-        <v>301721.9088</v>
+        <v>311352.2643</v>
       </c>
       <c r="G33">
-        <v>24232.2302</v>
+        <v>26406.9175</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -3230,13 +3326,13 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <v>27181.54</v>
+        <v>34725.64</v>
       </c>
       <c r="N33">
-        <v>270393.7</v>
+        <v>314368.92</v>
       </c>
       <c r="O33">
-        <v>22089.34</v>
+        <v>0</v>
       </c>
       <c r="P33">
         <v>0</v>
@@ -3254,13 +3350,13 @@
         <v>0</v>
       </c>
       <c r="U33">
-        <v>27181.54</v>
+        <v>34725.64</v>
       </c>
       <c r="V33">
-        <v>270393.7</v>
+        <v>314368.92</v>
       </c>
       <c r="W33">
-        <v>22089.34</v>
+        <v>0</v>
       </c>
       <c r="X33">
         <v>0</v>
@@ -3278,12 +3374,12 @@
         <v>0</v>
       </c>
       <c r="AC33">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="1">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
@@ -3292,13 +3388,13 @@
         <v>2025</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="E34">
-        <v>30000</v>
+        <v>20558.98</v>
       </c>
       <c r="F34">
-        <v>120000</v>
+        <v>300178.145</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -3307,22 +3403,22 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <v>70000</v>
+        <v>0</v>
       </c>
       <c r="J34">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="K34">
         <v>0</v>
       </c>
       <c r="L34">
-        <v>22674.42</v>
+        <v>0</v>
       </c>
       <c r="M34">
-        <v>81189.56</v>
+        <v>35983.12</v>
       </c>
       <c r="N34">
-        <v>75026.78</v>
+        <v>297098.25</v>
       </c>
       <c r="O34">
         <v>0</v>
@@ -3334,7 +3430,7 @@
         <v>0</v>
       </c>
       <c r="R34">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="S34">
         <v>0</v>
@@ -3343,10 +3439,10 @@
         <v>0</v>
       </c>
       <c r="U34">
-        <v>81189.56</v>
+        <v>35983.12</v>
       </c>
       <c r="V34">
-        <v>75026.78</v>
+        <v>297098.25</v>
       </c>
       <c r="W34">
         <v>0</v>
@@ -3358,7 +3454,7 @@
         <v>0</v>
       </c>
       <c r="Z34">
-        <v>0</v>
+        <v>36493.87</v>
       </c>
       <c r="AA34">
         <v>0</v>
@@ -3367,12 +3463,12 @@
         <v>0</v>
       </c>
       <c r="AC34">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="1">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B35" t="s">
         <v>60</v>
@@ -3381,43 +3477,43 @@
         <v>2025</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>80000</v>
       </c>
       <c r="F35">
-        <v>433983.8522</v>
+        <v>120000</v>
       </c>
       <c r="G35">
-        <v>66756.6691</v>
+        <v>0</v>
       </c>
       <c r="H35">
-        <v>37362.8604</v>
+        <v>0</v>
       </c>
       <c r="I35">
-        <v>10000</v>
+        <v>35000</v>
       </c>
       <c r="J35">
         <v>0</v>
       </c>
       <c r="K35">
-        <v>110048.5105</v>
+        <v>0</v>
       </c>
       <c r="L35">
-        <v>0</v>
+        <v>22674.42</v>
       </c>
       <c r="M35">
-        <v>33875.99</v>
+        <v>52083.67</v>
       </c>
       <c r="N35">
-        <v>388449.69</v>
+        <v>166132.1</v>
       </c>
       <c r="O35">
-        <v>41728.31</v>
+        <v>0</v>
       </c>
       <c r="P35">
-        <v>34125.23</v>
+        <v>0</v>
       </c>
       <c r="Q35">
         <v>0</v>
@@ -3432,16 +3528,16 @@
         <v>0</v>
       </c>
       <c r="U35">
-        <v>33875.99</v>
+        <v>52083.67</v>
       </c>
       <c r="V35">
-        <v>388449.69</v>
+        <v>166132.1</v>
       </c>
       <c r="W35">
-        <v>41728.31</v>
+        <v>0</v>
       </c>
       <c r="X35">
-        <v>34125.23</v>
+        <v>0</v>
       </c>
       <c r="Y35">
         <v>0</v>
@@ -3456,12 +3552,12 @@
         <v>0</v>
       </c>
       <c r="AC35">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="1">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
         <v>61</v>
@@ -3470,19 +3566,19 @@
         <v>2025</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="E36">
-        <v>19881.64</v>
+        <v>14668.56</v>
       </c>
       <c r="F36">
-        <v>544086.7781999999</v>
+        <v>301721.9088</v>
       </c>
       <c r="G36">
-        <v>0</v>
+        <v>24232.2302</v>
       </c>
       <c r="H36">
-        <v>34335.4349</v>
+        <v>0</v>
       </c>
       <c r="I36">
         <v>0</v>
@@ -3497,16 +3593,16 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <v>24492.98</v>
+        <v>27181.54</v>
       </c>
       <c r="N36">
-        <v>532274.26</v>
+        <v>270393.7</v>
       </c>
       <c r="O36">
-        <v>0</v>
+        <v>22089.34</v>
       </c>
       <c r="P36">
-        <v>13669.61</v>
+        <v>0</v>
       </c>
       <c r="Q36">
         <v>0</v>
@@ -3521,16 +3617,16 @@
         <v>0</v>
       </c>
       <c r="U36">
-        <v>24492.98</v>
+        <v>27181.54</v>
       </c>
       <c r="V36">
-        <v>532274.26</v>
+        <v>270393.7</v>
       </c>
       <c r="W36">
-        <v>0</v>
+        <v>22089.34</v>
       </c>
       <c r="X36">
-        <v>13669.61</v>
+        <v>0</v>
       </c>
       <c r="Y36">
         <v>0</v>
@@ -3545,12 +3641,12 @@
         <v>0</v>
       </c>
       <c r="AC36">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="1">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B37" t="s">
         <v>62</v>
@@ -3559,22 +3655,22 @@
         <v>2025</v>
       </c>
       <c r="D37" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E37">
-        <v>20006.44</v>
+        <v>30000</v>
       </c>
       <c r="F37">
-        <v>386492.0891</v>
+        <v>120000</v>
       </c>
       <c r="G37">
-        <v>26973.826</v>
+        <v>0</v>
       </c>
       <c r="H37">
         <v>0</v>
       </c>
       <c r="I37">
-        <v>0</v>
+        <v>70000</v>
       </c>
       <c r="J37">
         <v>0</v>
@@ -3583,16 +3679,40 @@
         <v>0</v>
       </c>
       <c r="L37">
-        <v>0</v>
+        <v>22674.42</v>
+      </c>
+      <c r="M37">
+        <v>81189.56</v>
+      </c>
+      <c r="N37">
+        <v>75026.78</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+      <c r="P37">
+        <v>0</v>
+      </c>
+      <c r="Q37">
+        <v>0</v>
+      </c>
+      <c r="R37">
+        <v>0</v>
+      </c>
+      <c r="S37">
+        <v>0</v>
+      </c>
+      <c r="T37">
+        <v>21490.444</v>
       </c>
       <c r="U37">
-        <v>20006.44</v>
+        <v>81189.56</v>
       </c>
       <c r="V37">
-        <v>386492.0891</v>
+        <v>75026.78</v>
       </c>
       <c r="W37">
-        <v>26973.826</v>
+        <v>0</v>
       </c>
       <c r="X37">
         <v>0</v>
@@ -3606,13 +3726,16 @@
       <c r="AA37">
         <v>0</v>
       </c>
+      <c r="AB37">
+        <v>21490.444</v>
+      </c>
       <c r="AC37">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="1">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B38" t="s">
         <v>63</v>
@@ -3621,43 +3744,43 @@
         <v>2025</v>
       </c>
       <c r="D38" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E38">
-        <v>32773.06</v>
+        <v>0</v>
       </c>
       <c r="F38">
-        <v>341581.165</v>
+        <v>433983.8522</v>
       </c>
       <c r="G38">
-        <v>0</v>
+        <v>66756.6691</v>
       </c>
       <c r="H38">
-        <v>36550.6243</v>
+        <v>37362.8604</v>
       </c>
       <c r="I38">
-        <v>15000</v>
+        <v>10000</v>
       </c>
       <c r="J38">
         <v>0</v>
       </c>
       <c r="K38">
-        <v>0</v>
+        <v>110048.5105</v>
       </c>
       <c r="L38">
         <v>0</v>
       </c>
       <c r="M38">
-        <v>35046.84</v>
+        <v>33875.99</v>
       </c>
       <c r="N38">
-        <v>349849.48</v>
+        <v>388449.69</v>
       </c>
       <c r="O38">
-        <v>11417</v>
+        <v>41728.31</v>
       </c>
       <c r="P38">
-        <v>36470.26</v>
+        <v>34125.23</v>
       </c>
       <c r="Q38">
         <v>0</v>
@@ -3672,16 +3795,16 @@
         <v>0</v>
       </c>
       <c r="U38">
-        <v>35046.84</v>
+        <v>33875.99</v>
       </c>
       <c r="V38">
-        <v>349849.48</v>
+        <v>388449.69</v>
       </c>
       <c r="W38">
-        <v>11417</v>
+        <v>41728.31</v>
       </c>
       <c r="X38">
-        <v>36470.26</v>
+        <v>34125.23</v>
       </c>
       <c r="Y38">
         <v>0</v>
@@ -3701,7 +3824,7 @@
     </row>
     <row r="39" spans="1:29">
       <c r="A39" s="1">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B39" t="s">
         <v>64</v>
@@ -3710,19 +3833,19 @@
         <v>2025</v>
       </c>
       <c r="D39" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E39">
-        <v>29792.44</v>
+        <v>19881.64</v>
       </c>
       <c r="F39">
-        <v>592371.3167</v>
+        <v>544086.7781999999</v>
       </c>
       <c r="G39">
-        <v>25940.9131</v>
+        <v>0</v>
       </c>
       <c r="H39">
-        <v>37196.7212</v>
+        <v>34335.4349</v>
       </c>
       <c r="I39">
         <v>0</v>
@@ -3734,22 +3857,22 @@
         <v>0</v>
       </c>
       <c r="L39">
-        <v>500373.46</v>
+        <v>0</v>
       </c>
       <c r="M39">
-        <v>35571.27</v>
+        <v>24492.98</v>
       </c>
       <c r="N39">
-        <v>48616.23</v>
+        <v>532274.26</v>
       </c>
       <c r="O39">
-        <v>37765.32</v>
+        <v>0</v>
       </c>
       <c r="P39">
-        <v>37083.02</v>
+        <v>13669.61</v>
       </c>
       <c r="Q39">
-        <v>26413.08</v>
+        <v>0</v>
       </c>
       <c r="R39">
         <v>0</v>
@@ -3758,22 +3881,22 @@
         <v>0</v>
       </c>
       <c r="T39">
-        <v>500373.46</v>
+        <v>0</v>
       </c>
       <c r="U39">
-        <v>35571.27</v>
+        <v>24492.98</v>
       </c>
       <c r="V39">
-        <v>48616.23</v>
+        <v>532274.26</v>
       </c>
       <c r="W39">
-        <v>37765.32</v>
+        <v>0</v>
       </c>
       <c r="X39">
-        <v>37083.02</v>
+        <v>13669.61</v>
       </c>
       <c r="Y39">
-        <v>26413.08</v>
+        <v>0</v>
       </c>
       <c r="Z39">
         <v>0</v>
@@ -3782,15 +3905,15 @@
         <v>0</v>
       </c>
       <c r="AB39">
-        <v>500373.46</v>
+        <v>0</v>
       </c>
       <c r="AC39">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="1">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
         <v>65</v>
@@ -3799,16 +3922,16 @@
         <v>2025</v>
       </c>
       <c r="D40" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="E40">
-        <v>0</v>
+        <v>20006.44</v>
       </c>
       <c r="F40">
-        <v>0</v>
+        <v>386492.0891</v>
       </c>
       <c r="G40">
-        <v>0</v>
+        <v>26973.826</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -3825,38 +3948,14 @@
       <c r="L40">
         <v>0</v>
       </c>
-      <c r="M40">
-        <v>0</v>
-      </c>
-      <c r="N40">
-        <v>0</v>
-      </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-      <c r="P40">
-        <v>0</v>
-      </c>
-      <c r="Q40">
-        <v>0</v>
-      </c>
-      <c r="R40">
-        <v>0</v>
-      </c>
-      <c r="S40">
-        <v>0</v>
-      </c>
-      <c r="T40">
-        <v>0</v>
-      </c>
       <c r="U40">
-        <v>0</v>
+        <v>20006.44</v>
       </c>
       <c r="V40">
-        <v>0</v>
+        <v>386492.0891</v>
       </c>
       <c r="W40">
-        <v>0</v>
+        <v>26973.826</v>
       </c>
       <c r="X40">
         <v>0</v>
@@ -3870,16 +3969,13 @@
       <c r="AA40">
         <v>0</v>
       </c>
-      <c r="AB40">
-        <v>0</v>
-      </c>
       <c r="AC40">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:29">
       <c r="A41" s="1">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B41" t="s">
         <v>66</v>
@@ -3891,19 +3987,19 @@
         <v>79</v>
       </c>
       <c r="E41">
-        <v>0</v>
+        <v>32773.06</v>
       </c>
       <c r="F41">
-        <v>0</v>
+        <v>341581.165</v>
       </c>
       <c r="G41">
         <v>0</v>
       </c>
       <c r="H41">
-        <v>0</v>
+        <v>36550.6243</v>
       </c>
       <c r="I41">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="J41">
         <v>0</v>
@@ -3914,17 +4010,41 @@
       <c r="L41">
         <v>0</v>
       </c>
+      <c r="M41">
+        <v>35046.84</v>
+      </c>
+      <c r="N41">
+        <v>349849.48</v>
+      </c>
+      <c r="O41">
+        <v>11417</v>
+      </c>
+      <c r="P41">
+        <v>36470.26</v>
+      </c>
+      <c r="Q41">
+        <v>0</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41">
+        <v>0</v>
+      </c>
+      <c r="T41">
+        <v>0</v>
+      </c>
       <c r="U41">
-        <v>0</v>
+        <v>35046.84</v>
       </c>
       <c r="V41">
-        <v>0</v>
+        <v>349849.48</v>
       </c>
       <c r="W41">
-        <v>0</v>
+        <v>11417</v>
       </c>
       <c r="X41">
-        <v>0</v>
+        <v>36470.26</v>
       </c>
       <c r="Y41">
         <v>0</v>
@@ -3935,13 +4055,16 @@
       <c r="AA41">
         <v>0</v>
       </c>
+      <c r="AB41">
+        <v>0</v>
+      </c>
       <c r="AC41">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="1">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
         <v>67</v>
@@ -3950,19 +4073,19 @@
         <v>2025</v>
       </c>
       <c r="D42" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E42">
-        <v>25326.82</v>
+        <v>29792.44</v>
       </c>
       <c r="F42">
-        <v>276375.5386</v>
+        <v>592371.3167</v>
       </c>
       <c r="G42">
-        <v>25008.9042</v>
+        <v>25940.9131</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>37196.7212</v>
       </c>
       <c r="I42">
         <v>0</v>
@@ -3974,22 +4097,22 @@
         <v>0</v>
       </c>
       <c r="L42">
-        <v>23876.1125</v>
+        <v>500373.46</v>
       </c>
       <c r="M42">
-        <v>27944</v>
+        <v>35571.27</v>
       </c>
       <c r="N42">
-        <v>230888.76</v>
+        <v>48616.23</v>
       </c>
       <c r="O42">
-        <v>0</v>
+        <v>37765.32</v>
       </c>
       <c r="P42">
-        <v>0</v>
+        <v>37083.02</v>
       </c>
       <c r="Q42">
-        <v>0</v>
+        <v>26413.08</v>
       </c>
       <c r="R42">
         <v>0</v>
@@ -3998,22 +4121,22 @@
         <v>0</v>
       </c>
       <c r="T42">
-        <v>23876.1125</v>
+        <v>500373.46</v>
       </c>
       <c r="U42">
-        <v>27944</v>
+        <v>35571.27</v>
       </c>
       <c r="V42">
-        <v>230888.76</v>
+        <v>48616.23</v>
       </c>
       <c r="W42">
-        <v>0</v>
+        <v>37765.32</v>
       </c>
       <c r="X42">
-        <v>0</v>
+        <v>37083.02</v>
       </c>
       <c r="Y42">
-        <v>0</v>
+        <v>26413.08</v>
       </c>
       <c r="Z42">
         <v>0</v>
@@ -4022,15 +4145,15 @@
         <v>0</v>
       </c>
       <c r="AB42">
-        <v>23876.1125</v>
+        <v>500373.46</v>
       </c>
       <c r="AC42">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="1">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
         <v>68</v>
@@ -4039,19 +4162,19 @@
         <v>2025</v>
       </c>
       <c r="D43" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E43">
-        <v>18541.06</v>
+        <v>0</v>
       </c>
       <c r="F43">
-        <v>252067.7995</v>
+        <v>0</v>
       </c>
       <c r="G43">
-        <v>26979.2036</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>36919.8225</v>
+        <v>0</v>
       </c>
       <c r="I43">
         <v>0</v>
@@ -4060,19 +4183,19 @@
         <v>0</v>
       </c>
       <c r="K43">
-        <v>5600</v>
+        <v>0</v>
       </c>
       <c r="L43">
-        <v>52444.52</v>
+        <v>0</v>
       </c>
       <c r="M43">
-        <v>28895.31</v>
+        <v>0</v>
       </c>
       <c r="N43">
-        <v>251643.6000000001</v>
+        <v>0</v>
       </c>
       <c r="O43">
-        <v>3379</v>
+        <v>0</v>
       </c>
       <c r="P43">
         <v>0</v>
@@ -4084,19 +4207,19 @@
         <v>0</v>
       </c>
       <c r="S43">
-        <v>8029.89</v>
+        <v>0</v>
       </c>
       <c r="T43">
-        <v>52444.52</v>
+        <v>0</v>
       </c>
       <c r="U43">
-        <v>28895.31</v>
+        <v>0</v>
       </c>
       <c r="V43">
-        <v>251643.6000000001</v>
+        <v>0</v>
       </c>
       <c r="W43">
-        <v>3379</v>
+        <v>0</v>
       </c>
       <c r="X43">
         <v>0</v>
@@ -4108,18 +4231,18 @@
         <v>0</v>
       </c>
       <c r="AA43">
-        <v>8029.89</v>
+        <v>0</v>
       </c>
       <c r="AB43">
-        <v>52444.52</v>
+        <v>0</v>
       </c>
       <c r="AC43">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:29">
       <c r="A44" s="1">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
         <v>69</v>
@@ -4128,19 +4251,19 @@
         <v>2025</v>
       </c>
       <c r="D44" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="E44">
-        <v>21854.46</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>624821.7819000001</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>12116.1151</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>40316.4462</v>
+        <v>0</v>
       </c>
       <c r="I44">
         <v>0</v>
@@ -4149,46 +4272,22 @@
         <v>0</v>
       </c>
       <c r="K44">
-        <v>19487.5781</v>
+        <v>0</v>
       </c>
       <c r="L44">
-        <v>229812.833425</v>
-      </c>
-      <c r="M44">
-        <v>29071.03</v>
-      </c>
-      <c r="N44">
-        <v>325344.86</v>
-      </c>
-      <c r="O44">
-        <v>91485.00999999999</v>
-      </c>
-      <c r="P44">
-        <v>39357.69</v>
-      </c>
-      <c r="Q44">
-        <v>0</v>
-      </c>
-      <c r="R44">
-        <v>0</v>
-      </c>
-      <c r="S44">
-        <v>63566</v>
-      </c>
-      <c r="T44">
-        <v>229812.833425</v>
+        <v>0</v>
       </c>
       <c r="U44">
-        <v>29071.03</v>
+        <v>0</v>
       </c>
       <c r="V44">
-        <v>325344.86</v>
+        <v>0</v>
       </c>
       <c r="W44">
-        <v>91485.00999999999</v>
+        <v>0</v>
       </c>
       <c r="X44">
-        <v>39357.69</v>
+        <v>0</v>
       </c>
       <c r="Y44">
         <v>0</v>
@@ -4197,18 +4296,15 @@
         <v>0</v>
       </c>
       <c r="AA44">
-        <v>63566</v>
-      </c>
-      <c r="AB44">
-        <v>229812.833425</v>
+        <v>0</v>
       </c>
       <c r="AC44">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="1">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
@@ -4220,78 +4316,407 @@
         <v>75</v>
       </c>
       <c r="E45">
+        <v>23898.82</v>
+      </c>
+      <c r="F45">
+        <v>409625.5938</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>32674.0429</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>42006.49</v>
+      </c>
+      <c r="U45">
+        <v>23898.82</v>
+      </c>
+      <c r="V45">
+        <v>409625.5938</v>
+      </c>
+      <c r="W45">
+        <v>0</v>
+      </c>
+      <c r="X45">
+        <v>32674.0429</v>
+      </c>
+      <c r="Y45">
+        <v>0</v>
+      </c>
+      <c r="Z45">
+        <v>0</v>
+      </c>
+      <c r="AA45">
+        <v>0</v>
+      </c>
+      <c r="AC45">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:29">
+      <c r="A46" s="1">
+        <v>47</v>
+      </c>
+      <c r="B46" t="s">
+        <v>71</v>
+      </c>
+      <c r="C46">
+        <v>2025</v>
+      </c>
+      <c r="D46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E46">
+        <v>25326.82</v>
+      </c>
+      <c r="F46">
+        <v>276375.5386</v>
+      </c>
+      <c r="G46">
+        <v>25008.9042</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>0</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>0</v>
+      </c>
+      <c r="L46">
+        <v>23876.1125</v>
+      </c>
+      <c r="M46">
+        <v>27944</v>
+      </c>
+      <c r="N46">
+        <v>230888.76</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="Q46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>23876.1125</v>
+      </c>
+      <c r="U46">
+        <v>27944</v>
+      </c>
+      <c r="V46">
+        <v>230888.76</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46">
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>0</v>
+      </c>
+      <c r="Z46">
+        <v>0</v>
+      </c>
+      <c r="AA46">
+        <v>0</v>
+      </c>
+      <c r="AB46">
+        <v>23876.1125</v>
+      </c>
+      <c r="AC46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:29">
+      <c r="A47" s="1">
+        <v>48</v>
+      </c>
+      <c r="B47" t="s">
+        <v>72</v>
+      </c>
+      <c r="C47">
+        <v>2025</v>
+      </c>
+      <c r="D47" t="s">
+        <v>80</v>
+      </c>
+      <c r="E47">
+        <v>18541.06</v>
+      </c>
+      <c r="F47">
+        <v>252067.7995</v>
+      </c>
+      <c r="G47">
+        <v>26979.2036</v>
+      </c>
+      <c r="H47">
+        <v>36919.8225</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>0</v>
+      </c>
+      <c r="K47">
+        <v>5600</v>
+      </c>
+      <c r="L47">
+        <v>52444.52</v>
+      </c>
+      <c r="M47">
+        <v>28895.31</v>
+      </c>
+      <c r="N47">
+        <v>251643.6000000001</v>
+      </c>
+      <c r="O47">
+        <v>3379</v>
+      </c>
+      <c r="P47">
+        <v>0</v>
+      </c>
+      <c r="Q47">
+        <v>0</v>
+      </c>
+      <c r="R47">
+        <v>0</v>
+      </c>
+      <c r="S47">
+        <v>8029.89</v>
+      </c>
+      <c r="T47">
+        <v>52444.52</v>
+      </c>
+      <c r="U47">
+        <v>28895.31</v>
+      </c>
+      <c r="V47">
+        <v>251643.6000000001</v>
+      </c>
+      <c r="W47">
+        <v>3379</v>
+      </c>
+      <c r="X47">
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>0</v>
+      </c>
+      <c r="Z47">
+        <v>0</v>
+      </c>
+      <c r="AA47">
+        <v>8029.89</v>
+      </c>
+      <c r="AB47">
+        <v>52444.52</v>
+      </c>
+      <c r="AC47">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:29">
+      <c r="A48" s="1">
+        <v>49</v>
+      </c>
+      <c r="B48" t="s">
+        <v>73</v>
+      </c>
+      <c r="C48">
+        <v>2025</v>
+      </c>
+      <c r="D48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48">
+        <v>21854.46</v>
+      </c>
+      <c r="F48">
+        <v>624821.7819000001</v>
+      </c>
+      <c r="G48">
+        <v>12116.1151</v>
+      </c>
+      <c r="H48">
+        <v>40316.4462</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>19487.5781</v>
+      </c>
+      <c r="L48">
+        <v>229812.833425</v>
+      </c>
+      <c r="M48">
+        <v>33879.14</v>
+      </c>
+      <c r="N48">
+        <v>325344.86</v>
+      </c>
+      <c r="O48">
+        <v>91485.00999999999</v>
+      </c>
+      <c r="P48">
+        <v>39357.69</v>
+      </c>
+      <c r="Q48">
+        <v>0</v>
+      </c>
+      <c r="R48">
+        <v>0</v>
+      </c>
+      <c r="S48">
+        <v>63566</v>
+      </c>
+      <c r="T48">
+        <v>229812.833425</v>
+      </c>
+      <c r="U48">
+        <v>33879.14</v>
+      </c>
+      <c r="V48">
+        <v>325344.86</v>
+      </c>
+      <c r="W48">
+        <v>91485.00999999999</v>
+      </c>
+      <c r="X48">
+        <v>39357.69</v>
+      </c>
+      <c r="Y48">
+        <v>0</v>
+      </c>
+      <c r="Z48">
+        <v>0</v>
+      </c>
+      <c r="AA48">
+        <v>63566</v>
+      </c>
+      <c r="AB48">
+        <v>229812.833425</v>
+      </c>
+      <c r="AC48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29">
+      <c r="A49" s="1">
+        <v>50</v>
+      </c>
+      <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49">
+        <v>2025</v>
+      </c>
+      <c r="D49" t="s">
+        <v>80</v>
+      </c>
+      <c r="E49">
         <v>27683.86</v>
       </c>
-      <c r="F45">
+      <c r="F49">
         <v>418982.5319</v>
       </c>
-      <c r="G45">
+      <c r="G49">
         <v>51527.9349</v>
       </c>
-      <c r="H45">
+      <c r="H49">
         <v>40992.0789</v>
       </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>0</v>
-      </c>
-      <c r="K45">
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>0</v>
+      </c>
+      <c r="K49">
         <v>181185.5419</v>
       </c>
-      <c r="L45">
+      <c r="L49">
         <v>60577.37</v>
       </c>
-      <c r="M45">
+      <c r="M49">
         <v>30868.28</v>
       </c>
-      <c r="N45">
+      <c r="N49">
         <v>363209.57</v>
       </c>
-      <c r="O45">
+      <c r="O49">
         <v>65966.92</v>
       </c>
-      <c r="P45">
-        <v>0</v>
-      </c>
-      <c r="Q45">
-        <v>0</v>
-      </c>
-      <c r="R45">
-        <v>0</v>
-      </c>
-      <c r="S45">
+      <c r="P49">
+        <v>0</v>
+      </c>
+      <c r="Q49">
+        <v>0</v>
+      </c>
+      <c r="R49">
+        <v>0</v>
+      </c>
+      <c r="S49">
         <v>95933.12</v>
       </c>
-      <c r="T45">
+      <c r="T49">
         <v>60577.37</v>
       </c>
-      <c r="U45">
+      <c r="U49">
         <v>30868.28</v>
       </c>
-      <c r="V45">
+      <c r="V49">
         <v>363209.57</v>
       </c>
-      <c r="W45">
+      <c r="W49">
         <v>65966.92</v>
       </c>
-      <c r="X45">
-        <v>0</v>
-      </c>
-      <c r="Y45">
-        <v>0</v>
-      </c>
-      <c r="Z45">
-        <v>0</v>
-      </c>
-      <c r="AA45">
+      <c r="X49">
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>0</v>
+      </c>
+      <c r="Z49">
+        <v>0</v>
+      </c>
+      <c r="AA49">
         <v>95933.12</v>
       </c>
-      <c r="AB45">
+      <c r="AB49">
         <v>60577.37</v>
       </c>
-      <c r="AC45">
+      <c r="AC49">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios Año y Catalogos
</commit_message>
<xml_diff>
--- a/als-salida.xlsx
+++ b/als-salida.xlsx
@@ -755,14 +755,38 @@
       <c r="L2">
         <v>0</v>
       </c>
+      <c r="M2">
+        <v>13391.57</v>
+      </c>
+      <c r="N2">
+        <v>279350.01</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>63774.22</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
       <c r="U2">
-        <v>12973.06</v>
+        <v>13391.57</v>
       </c>
       <c r="V2">
-        <v>302399.9252000001</v>
+        <v>279350.01</v>
       </c>
       <c r="W2">
-        <v>10239.5255</v>
+        <v>0</v>
       </c>
       <c r="X2">
         <v>0</v>
@@ -774,6 +798,9 @@
         <v>0</v>
       </c>
       <c r="AA2">
+        <v>63774.22</v>
+      </c>
+      <c r="AB2">
         <v>0</v>
       </c>
       <c r="AC2">
@@ -879,14 +906,38 @@
       <c r="L4">
         <v>0</v>
       </c>
+      <c r="M4">
+        <v>33666.72</v>
+      </c>
+      <c r="N4">
+        <v>341703.8</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
       <c r="U4">
-        <v>18205.06</v>
+        <v>33666.72</v>
       </c>
       <c r="V4">
-        <v>324144.4391</v>
+        <v>341703.8</v>
       </c>
       <c r="W4">
-        <v>25164.239</v>
+        <v>0</v>
       </c>
       <c r="X4">
         <v>0</v>
@@ -898,6 +949,9 @@
         <v>0</v>
       </c>
       <c r="AA4">
+        <v>0</v>
+      </c>
+      <c r="AB4">
         <v>0</v>
       </c>
       <c r="AC4">
@@ -1413,7 +1467,7 @@
     </row>
     <row r="11" spans="1:29">
       <c r="A11" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>37</v>
@@ -1502,7 +1556,7 @@
     </row>
     <row r="12" spans="1:29">
       <c r="A12" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>38</v>
@@ -1591,7 +1645,7 @@
     </row>
     <row r="13" spans="1:29">
       <c r="A13" s="1">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" t="s">
         <v>39</v>
@@ -1680,7 +1734,7 @@
     </row>
     <row r="14" spans="1:29">
       <c r="A14" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
@@ -1719,7 +1773,7 @@
         <v>24406.71</v>
       </c>
       <c r="N14">
-        <v>340968.83</v>
+        <v>334593.33</v>
       </c>
       <c r="O14">
         <v>5162.22</v>
@@ -1743,7 +1797,7 @@
         <v>24406.71</v>
       </c>
       <c r="V14">
-        <v>340968.83</v>
+        <v>334593.33</v>
       </c>
       <c r="W14">
         <v>5162.22</v>
@@ -1769,7 +1823,7 @@
     </row>
     <row r="15" spans="1:29">
       <c r="A15" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>41</v>
@@ -1858,7 +1912,7 @@
     </row>
     <row r="16" spans="1:29">
       <c r="A16" s="1">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
         <v>42</v>
@@ -1947,7 +2001,7 @@
     </row>
     <row r="17" spans="1:29">
       <c r="A17" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B17" t="s">
         <v>42</v>
@@ -2036,7 +2090,7 @@
     </row>
     <row r="18" spans="1:29">
       <c r="A18" s="1">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B18" t="s">
         <v>43</v>
@@ -2125,7 +2179,7 @@
     </row>
     <row r="19" spans="1:29">
       <c r="A19" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
         <v>44</v>
@@ -2214,7 +2268,7 @@
     </row>
     <row r="20" spans="1:29">
       <c r="A20" s="1">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
         <v>45</v>
@@ -2303,7 +2357,7 @@
     </row>
     <row r="21" spans="1:29">
       <c r="A21" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
         <v>46</v>
@@ -2392,7 +2446,7 @@
     </row>
     <row r="22" spans="1:29">
       <c r="A22" s="1">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
@@ -2454,7 +2508,7 @@
     </row>
     <row r="23" spans="1:29">
       <c r="A23" s="1">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>48</v>
@@ -2516,7 +2570,7 @@
     </row>
     <row r="24" spans="1:29">
       <c r="A24" s="1">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>49</v>
@@ -2605,7 +2659,7 @@
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="1">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>50</v>
@@ -2694,7 +2748,7 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="1">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>51</v>
@@ -2756,7 +2810,7 @@
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="1">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
@@ -2845,7 +2899,7 @@
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="1">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
         <v>53</v>
@@ -2934,7 +2988,7 @@
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="1">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B29" t="s">
         <v>54</v>
@@ -3023,7 +3077,7 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="1">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B30" t="s">
         <v>55</v>
@@ -3112,7 +3166,7 @@
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="1">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>56</v>
@@ -3201,7 +3255,7 @@
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="1">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B32" t="s">
         <v>57</v>
@@ -3290,7 +3344,7 @@
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>58</v>
@@ -3379,7 +3433,7 @@
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="1">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B34" t="s">
         <v>59</v>
@@ -3468,7 +3522,7 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="1">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
         <v>60</v>
@@ -3557,7 +3611,7 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="1">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B36" t="s">
         <v>61</v>
@@ -3646,7 +3700,7 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="1">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
         <v>62</v>
@@ -3735,7 +3789,7 @@
     </row>
     <row r="38" spans="1:29">
       <c r="A38" s="1">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B38" t="s">
         <v>63</v>
@@ -3824,7 +3878,7 @@
     </row>
     <row r="39" spans="1:29">
       <c r="A39" s="1">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B39" t="s">
         <v>64</v>
@@ -3913,7 +3967,7 @@
     </row>
     <row r="40" spans="1:29">
       <c r="A40" s="1">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B40" t="s">
         <v>65</v>
@@ -3975,7 +4029,7 @@
     </row>
     <row r="41" spans="1:29">
       <c r="A41" s="1">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B41" t="s">
         <v>66</v>
@@ -4064,7 +4118,7 @@
     </row>
     <row r="42" spans="1:29">
       <c r="A42" s="1">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B42" t="s">
         <v>67</v>
@@ -4153,7 +4207,7 @@
     </row>
     <row r="43" spans="1:29">
       <c r="A43" s="1">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
         <v>68</v>
@@ -4242,7 +4296,7 @@
     </row>
     <row r="44" spans="1:29">
       <c r="A44" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B44" t="s">
         <v>69</v>
@@ -4304,7 +4358,7 @@
     </row>
     <row r="45" spans="1:29">
       <c r="A45" s="1">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B45" t="s">
         <v>70</v>
@@ -4337,19 +4391,43 @@
         <v>0</v>
       </c>
       <c r="L45">
-        <v>42006.49</v>
+        <v>74021.34</v>
+      </c>
+      <c r="M45">
+        <v>26512.21</v>
+      </c>
+      <c r="N45">
+        <v>337917.65</v>
+      </c>
+      <c r="O45">
+        <v>60888.94</v>
+      </c>
+      <c r="P45">
+        <v>0</v>
+      </c>
+      <c r="Q45">
+        <v>0</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>74021.34</v>
       </c>
       <c r="U45">
-        <v>23898.82</v>
+        <v>26512.21</v>
       </c>
       <c r="V45">
-        <v>409625.5938</v>
+        <v>337917.65</v>
       </c>
       <c r="W45">
-        <v>0</v>
+        <v>60888.94</v>
       </c>
       <c r="X45">
-        <v>32674.0429</v>
+        <v>0</v>
       </c>
       <c r="Y45">
         <v>0</v>
@@ -4359,6 +4437,9 @@
       </c>
       <c r="AA45">
         <v>0</v>
+      </c>
+      <c r="AB45">
+        <v>74021.34</v>
       </c>
       <c r="AC45">
         <v>10</v>
@@ -4366,7 +4447,7 @@
     </row>
     <row r="46" spans="1:29">
       <c r="A46" s="1">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B46" t="s">
         <v>71</v>
@@ -4455,7 +4536,7 @@
     </row>
     <row r="47" spans="1:29">
       <c r="A47" s="1">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B47" t="s">
         <v>72</v>
@@ -4544,7 +4625,7 @@
     </row>
     <row r="48" spans="1:29">
       <c r="A48" s="1">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B48" t="s">
         <v>73</v>
@@ -4633,7 +4714,7 @@
     </row>
     <row r="49" spans="1:29">
       <c r="A49" s="1">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B49" t="s">
         <v>74</v>
@@ -4669,7 +4750,7 @@
         <v>60577.37</v>
       </c>
       <c r="M49">
-        <v>30868.28</v>
+        <v>136868.28</v>
       </c>
       <c r="N49">
         <v>363209.57</v>
@@ -4693,7 +4774,7 @@
         <v>60577.37</v>
       </c>
       <c r="U49">
-        <v>30868.28</v>
+        <v>136868.28</v>
       </c>
       <c r="V49">
         <v>363209.57</v>

</xml_diff>